<commit_message>
feat: integrate useGuardRoute hook in multiple pages for enhanced route protection and access control
</commit_message>
<xml_diff>
--- a/public/templates/them_van_bang_mau.xlsx
+++ b/public/templates/them_van_bang_mau.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LuanVan2025\Thêm văn bằng\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF45B410-594B-4F5D-9823-4A8F986DEC18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7D9800-BD68-4F82-8438-46F2BA1093F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Mã số sinh viên</t>
   </si>
@@ -58,37 +58,25 @@
     <t>Địa điểm đào tạo</t>
   </si>
   <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Tp. Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>Số vào sổ</t>
+  </si>
+  <si>
+    <t>DH52110009</t>
+  </si>
+  <si>
+    <t>Xuất sắc</t>
+  </si>
+  <si>
     <t>Đào tạo từ xa</t>
   </si>
   <si>
-    <t>Cử nhân</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Giỏi</t>
-  </si>
-  <si>
     <t>Kỹ sư</t>
-  </si>
-  <si>
-    <t>Chính quy</t>
-  </si>
-  <si>
-    <t>Tp. Hồ Chí Minh</t>
-  </si>
-  <si>
-    <t>Số vào sổ</t>
-  </si>
-  <si>
-    <t>Khá</t>
-  </si>
-  <si>
-    <t>DH5003299</t>
-  </si>
-  <si>
-    <t>SV002</t>
   </si>
 </sst>
 </file>
@@ -479,20 +467,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.58203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.25" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.58203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="17.9140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.58203125" style="2" customWidth="1"/>
+    <col min="2" max="6" width="15.58203125" style="2" customWidth="1"/>
     <col min="7" max="7" width="12.4140625" style="2" customWidth="1"/>
     <col min="8" max="8" width="15.58203125" style="2" customWidth="1"/>
     <col min="9" max="9" width="23.6640625" style="2" customWidth="1"/>
@@ -533,7 +517,7 @@
         <v>3</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -541,16 +525,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F2" s="2">
         <v>2025</v>
@@ -559,57 +543,25 @@
         <v>4</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="J2" s="2">
-        <v>121331123</v>
+        <v>18284322123</v>
       </c>
       <c r="K2" s="1">
-        <v>2131623</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="2">
-        <v>2025</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" s="2">
-        <v>211212131</v>
-      </c>
-      <c r="K3" s="1">
-        <v>1867123</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="H9" s="2" t="s">
-        <v>14</v>
-      </c>
+        <v>2522231023</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H8" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I11" s="3"/>
@@ -629,23 +581,8 @@
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I17" s="3"/>
-    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="LUXO68hW2Ghqen9SZUeivmtf1kDANMZlLlLb7KkNbOrZR0KOODW8JoRbLRgoWcAvybGRQbD81QPRSM1QlHCXfg==" saltValue="68xBB3MTwIoSFoxSI7usTA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{0B35BAD7-EE52-4192-A8BA-43E6D766BC0C}">
-      <formula1>"Xuất sắc, Giỏi, Khá, Trung bình"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576" xr:uid="{9AFEE0C8-879B-49D3-8773-6AC38B4AD5D6}">
-      <formula1>"Kỹ sư, Cử nhân"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{E6516F61-7652-4723-9788-1147F1A237CB}">
-      <formula1>"Chính quy, Đào tạo từ xa"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: refactor user logout handling in NavUser and StudentTopbar components; replace useLogoutMutation with direct signOut call and improve loading state management
</commit_message>
<xml_diff>
--- a/public/templates/them_van_bang_mau.xlsx
+++ b/public/templates/them_van_bang_mau.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LuanVan2025\Thêm văn bằng\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HOANG\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7D9800-BD68-4F82-8438-46F2BA1093F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3028FB50-6890-4B4F-9194-9431F7CB6694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Mã số sinh viên</t>
   </si>
@@ -34,9 +34,6 @@
     <t>Số hiệu bằng</t>
   </si>
   <si>
-    <t>11/08/2025</t>
-  </si>
-  <si>
     <t>STT</t>
   </si>
   <si>
@@ -67,9 +64,6 @@
     <t>Số vào sổ</t>
   </si>
   <si>
-    <t>DH52110009</t>
-  </si>
-  <si>
     <t>Xuất sắc</t>
   </si>
   <si>
@@ -77,12 +71,18 @@
   </si>
   <si>
     <t>Kỹ sư</t>
+  </si>
+  <si>
+    <t>QE100006</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -147,7 +147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -162,6 +162,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -470,14 +477,14 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.33203125" style="2" customWidth="1"/>
     <col min="2" max="6" width="15.58203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.4140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.4140625" style="6" customWidth="1"/>
     <col min="8" max="8" width="15.58203125" style="2" customWidth="1"/>
     <col min="9" max="9" width="23.6640625" style="2" customWidth="1"/>
     <col min="10" max="10" width="15.58203125" style="2" customWidth="1"/>
@@ -487,28 +494,28 @@
   <sheetData>
     <row r="1" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>2</v>
@@ -517,7 +524,7 @@
         <v>3</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -525,39 +532,39 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="F2" s="2">
         <v>2025</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>4</v>
+      <c r="G2" s="6">
+        <v>45871</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J2" s="2">
-        <v>18284322123</v>
+        <v>3</v>
       </c>
       <c r="K2" s="1">
-        <v>2522231023</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>